<commit_message>
translate dq models to english
</commit_message>
<xml_diff>
--- a/dq_models/movie_ratings.xlsx
+++ b/dq_models/movie_ratings.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Documentos\GitHub\context-aware-dq-management-in-data-lakes\dq_models\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07B2976-D199-4CDE-8B64-C0BD04AD443C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="(Trusted Zone) movie_ratings.cs" sheetId="1" r:id="rId4"/>
+    <sheet name="(Trusted Zone) movie_ratings.cs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -34,296 +43,298 @@
     <t>Applied DQ Method</t>
   </si>
   <si>
+    <t>ID: AME24
+Applied to: movie_ratings.csv, “release_date”</t>
+  </si>
+  <si>
+    <t>ID: AME25
+Applied to: movie_ratings.csv, “title”</t>
+  </si>
+  <si>
+    <t>ID: AME26
+Applied to: movie_ratings.csv, “genres”</t>
+  </si>
+  <si>
+    <t>ID: AME27
+Applied to: movie_ratings.csv, “release_date”</t>
+  </si>
+  <si>
+    <t>ID: AME28
+Applied to: movie_ratings.csv, “vote_average”</t>
+  </si>
+  <si>
+    <t>ID: AME29
+Applied to: movie_ratings.csv, “vote_count”</t>
+  </si>
+  <si>
+    <t>ID: AME30
+Applied to: movie_ratings.csv, “production_countries”</t>
+  </si>
+  <si>
+    <t>ID: AME31
+Applied to: movie_ratings.csv</t>
+  </si>
+  <si>
+    <t>ID: AME32
+Applied to: movie_ratings.csv, “status”</t>
+  </si>
+  <si>
+    <t>ID: AME33
+Applied to: movie_ratings.csv, “vote_average”</t>
+  </si>
+  <si>
+    <t>ID: AME34
+Applied to: movie_ratings.csv, “vote_count”</t>
+  </si>
+  <si>
+    <t>ID: AME35
+Applied to: movie_ratings.csv, “id”</t>
+  </si>
+  <si>
+    <t>ID: AME36
+Applied to: movie_ratings.csv</t>
+  </si>
+  <si>
+    <t>ID: AME37
+Applied to: movie_ratings.csv</t>
+  </si>
+  <si>
     <t>ID: D1
 Name: 
-Exactitud
-Semantic: Concierne la correctitud y la precisión con que los datos del mundo real son representados en un sistema de información 
+Accuracy
+Semantic: It concerns the correctness and accuracy with which real-world data are represented in an information system. 
 Suggested by: {BR3}</t>
   </si>
   <si>
     <t>ID: D1F1
-Name: Exactitud 
-Sintáctica
-Semantic: Indica qué tan libre de errores sintácticos están los datos
+Name: Syntactic Accuracy
+Semantic: It indicates how free the data are from syntactic errors.
 Represents: {BR3}</t>
   </si>
   <si>
     <t>ID: M1
-Name: FormatoFecha
-Purpose: Mide si el formato de un dato que representa una fecha es correcto, relativo a un formato especificado.
-No se mide para datos faltantes.
+Name: DateFormat
+Purpose: It measures whether the format of a data value representing a date is correct, relative to a specified format.
+It is not measured for missing data.
 Influenced by: {BR3}
-Granularity: celda
+Granularity: cell
 Result domain: {0,1}</t>
   </si>
   <si>
     <t>ID: ME1 
-Name: verificarFormatoFecha
+Name: checkDateFormat
 Uses: {BR3} 
 Input data types: String, String
 Output data types: Boolean 
-Algorithm: verificarFormatoFecha(dato, formato)</t>
-  </si>
-  <si>
-    <t>ID: AME24
-Applied to: movie_ratings.csv, “release_date”</t>
+Algorithm: checkDateFormat(data, format)</t>
   </si>
   <si>
     <t>ID: D2
 Name: 
-Completitud
-Semantic: Concierne la proporción del mundo real que está representado en el SI
+Completeness
+Semantic: It concerns the proportion of the real world that is represented in the information system.
 Suggested by: {BR5, DL2}</t>
   </si>
   <si>
     <t>ID: D2F1
-Name: Densidad
-Semantic: Indica qué cantidad de registros con datos faltantes hay
+Name: Density
+Semantic: It indicates how many records contain missing data.
 Represents: {DL2}</t>
   </si>
   <si>
     <t>ID: M4
-Name: RatioNoVacios
-Purpose: Mide el grado de valores no faltantes en una columna. Lo que se considera faltante depende del método.
+Name: NonEmptyRatio
+Purpose:It measures the degree of non-missing values in a column. What is considered missing depends on the method.
 Influenced by: {DL2}
-Granularity: columna
+Granularity: column
 Result domain: [0..1]</t>
   </si>
   <si>
+    <t>ID: D2F2
+Name: Coverage
+Semantic: It indicates how much real-world data are represented in the system.
+Represents: {BR5}</t>
+  </si>
+  <si>
+    <t>ID: M5
+Name: CoveragePercentage
+Purpose: It measures the percentage of values that are represented by some record in the dataset, relative to a reference.
+Influenced by: {BR5}
+Granularity: dataset
+Result domain: [0..1]</t>
+  </si>
+  <si>
     <t>ID: ME4 
-Name: ratioNoNulos
+Name: nonNullRatio
 Uses: {DL2} 
 Input data types: Object[]
 Output data types: Float
-Algorithm: ratioNoNulos(columna)</t>
-  </si>
-  <si>
-    <t>ID: AME25
-Applied to: movie_ratings.csv, “title”</t>
-  </si>
-  <si>
-    <t>ID: AME26
-Applied to: movie_ratings.csv, “genres”</t>
-  </si>
-  <si>
-    <t>ID: AME27
-Applied to: movie_ratings.csv, “release_date”</t>
-  </si>
-  <si>
-    <t>ID: AME28
-Applied to: movie_ratings.csv, “vote_average”</t>
-  </si>
-  <si>
-    <t>ID: AME29
-Applied to: movie_ratings.csv, “vote_count”</t>
-  </si>
-  <si>
-    <t>ID: AME30
-Applied to: movie_ratings.csv, “production_countries”</t>
-  </si>
-  <si>
-    <t>ID: D2F2
-Name: Cobertura
-Semantic: Indica qué cantidad de datos de la realidad están representados en el sistema
-Represents: {BR5}</t>
-  </si>
-  <si>
-    <t>ID: M5
-Name: PorcentajeCobertura
-Purpose: Mide el porcentaje de valores que se encuentran representados por algún registro del dataset, relativo a un referencial
-Influenced by: {BR5}
-Granularity: dataset
-Result domain: [0..1]</t>
-  </si>
-  <si>
-    <t>ID: ME6 
-Name: porcentajeCoberturaRef
-Uses: {BR5}
-Input data types: Object[], String[]
-Output data types: Float
-Algorithm: porcentajeCoberturaRef(columna, ref)</t>
-  </si>
-  <si>
-    <t>ID: AME31
-Applied to: movie_ratings.csv</t>
+Algorithm: nonNullRatio(column)</t>
   </si>
   <si>
     <t>ID: D3
 Name: 
-Consistencia
-Semantic: Concierne la consistencia entre los registros del SI
+Consistency
+Semantic: It concerns the consistency among the records of the information system.
 Suggested by: {BR1, BR4, DL2}</t>
   </si>
   <si>
     <t>ID: D3F1
-Name: Integridad de Dominio
-Semantic: Indica que los datos representados estén en el dominio, dada su semántica y el dominio de aplicación
+Name: Domain Integrity
+Semantic: Indicates that the represented data fall within the domain, given their semantics and the application domain.
 Represents: {BR1, BR4, DL2}</t>
   </si>
   <si>
     <t>ID: M6
-Name: DatoEnDominioString
-Semantic: Mide si un dato de tipo texto es posible en el dominio, dado un referencial
+Name: DataInDomainString
+Semantic: It measures whether a text-type data value is valid within the domain, given a reference.
 Influenced by: {BR1}
-Granularity: celda
+Granularity: cell
 Result domain: {0,1}</t>
   </si>
   <si>
     <t>ID: ME7 
-Name: StatusEnDominio
-Semantic: Dado un dato y un referencial, verifica que el dato esté en el referencial
+Name: StatusInDomain
+Semantic: Given a data value and a reference, it checks whether the data value exists in the reference.
 Uses: {BR1} 
 Input data types: String, String[]
 Output data types: Boolean 
-Algorithm: verificarStatus(status, posiblesStatus)</t>
-  </si>
-  <si>
-    <t>ID: AME32
-Applied to: movie_ratings.csv, “status”</t>
+Algorithm: verifyStatus(status, posiblesStatus)</t>
   </si>
   <si>
     <t>ID: M7
-Name: DatoEnRango
-Semantic: Mide si un dato numérico es positivo
+Name: DataInRange
+Semantic: Measures if a numeric data is in a given range.
 Influenced by: {BR4, DL2}
-Granularity: celda
+Granularity: cell
 Result domain: {0,1}</t>
   </si>
   <si>
     <t>ID: ME8 
-Name: DatoEnRango
-Semantic: Dado un dato numérico, verifica si se encuentra en un rango dado
+Name: DataInRange
+Semantic: Given a numeric value, it checks whether it falls within a specified range.
 Uses: {BR4, DL2} 
 Input data types: Float, Float, Float
 Output data types: Boolean 
-Algorithm: verificarNumeroEnRango(dato)</t>
-  </si>
-  <si>
-    <t>ID: AME33
-Applied to: movie_ratings.csv, “vote_average”</t>
-  </si>
-  <si>
-    <t>ID: AME34
-Applied to: movie_ratings.csv, “vote_count”</t>
+Algorithm: verifyDataInRange(data)</t>
   </si>
   <si>
     <t>ID: D4
 Name: 
-Unicidad
-Semantic: Concierne el grado de repetición de los registros del SI
+Uniqueness
+Semantic: It concerns the degree of repetition of records in the information system.
 Suggested by: {DL2}</t>
   </si>
   <si>
     <t>ID: D4F1
-Name: No-Duplicación
-Semantic: Mide el grado de filas que son únicas
+Name: Non-Duplicity
+Semantic: It measures the proportion of rows that are unique.
 Arises from = {DL2}</t>
   </si>
   <si>
     <t>ID: M9
-Name: RatioClavesUnicas
-Semantic: Mide el grado de filas de un dataset que son únicas, según una fila identificadora
+Name: UniqueKeysRatio
+Semantic: It measures the proportion of rows in a dataset that are unique, based on an identifying row or key.
 Depends on = {DL2}
 Granularity: dataset
 Result domain: [0..1]</t>
   </si>
   <si>
-    <t>ID: ME10 
-Name: RatioClavesUnicas
-Uses: {DL2} 
-Input data types: Object[][], Object[]
-Output data types: Float
-Algorithm: ratioNoDupFilas(dataset, columna)</t>
-  </si>
-  <si>
-    <t>ID: AME35
-Applied to: movie_ratings.csv, “id”</t>
-  </si>
-  <si>
     <t>ID: D5
 Name: 
-Frescura
-Semantic: Concierne el grado en el que la edad de los datos afecta su uso
+Freshness
+Semantic: It concerns the degree to which the age of the data affects its use.
 Suggested by: {SR2}</t>
   </si>
   <si>
     <t>ID: D5F1
-Name: Oportunidad
-Semantic: Mide qué tan oportunos son los datos a la hora de su lectura
+Name: Timeliness
+Semantic: It measures how timely the data are at the time of reading.
 Represents: {SR2}</t>
   </si>
   <si>
     <t>ID: M10
-Name: OportunidadPuntaje
-Semantic: Calcula la diferencia en minutos entre la hora en la que se necesitan los datos y la hora en la que se actualizan
+Name: TimelinessScore
+Semantic: It calculates the difference in minutes between the time the data are needed and the time they are updated.
 Influenced by: {SR2}
 Granularity: dataset
 Result domain: [0..+inf)</t>
   </si>
   <si>
     <t>ID: ME13 
-Name: Oportunidad8:45am
+Name: Timeliness8:45am
 Uses: {SR2} 
 Input data types: Object[][]
 Output data types: Integer
 Algorithm: timelinessScore(dataset)</t>
   </si>
   <si>
-    <t>ID: AME36
-Applied to: movie_ratings.csv</t>
-  </si>
-  <si>
     <t>ID: M11
-Name: Edad
-Semantic: Calcula los minutos desde la última actualización de los datos
+Name: Staleness
+Semantic: It calculates the time since the data were last updated.
 Influenced by: {SR2}
 Granularity: dataset
 Result domain: [0..+inf)</t>
   </si>
   <si>
     <t>ID: ME12 
-Name: EdadMinutos
+Name: StalenessMinutes
 Uses: {SR2} 
 Input data types: Object[][]
 Output data types: Integer
 Algorithm: staleness(dataset)</t>
   </si>
   <si>
-    <t>ID: AME37
-Applied to: movie_ratings.csv</t>
+    <t>ID: ME6 
+Name: coveragePercentageRef
+Uses: {BR5}
+Input data types: Object[], String[]
+Output data types: Float
+Algorithm: coveragePercentageRef(column, ref)</t>
+  </si>
+  <si>
+    <t>ID: ME10 
+Name: UniqueKeysRatio
+Uses: {DL2} 
+Input data types: Object[][], Object[]
+Output data types: Float
+Algorithm: ratioNonDupRows(dataset, column)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Consolas"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -339,7 +350,13 @@
     </fill>
   </fills>
   <borders count="8">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
@@ -353,6 +370,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -367,6 +385,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -381,6 +400,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -392,6 +412,8 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -400,6 +422,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -408,9 +433,11 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -425,58 +452,63 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="7" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -666,255 +698,259 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="27.75"/>
-    <col customWidth="1" min="2" max="2" width="22.25"/>
-    <col customWidth="1" min="3" max="3" width="21.88"/>
-    <col customWidth="1" min="4" max="4" width="26.0"/>
-    <col customWidth="1" min="5" max="5" width="34.0"/>
+    <col min="1" max="1" width="27.73046875" customWidth="1"/>
+    <col min="2" max="2" width="22.265625" customWidth="1"/>
+    <col min="3" max="3" width="21.86328125" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4">
+    </row>
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" ht="91.5" customHeight="1">
+    <row r="5" spans="1:5" ht="91.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
     </row>
-    <row r="6">
-      <c r="A6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7">
+    <row r="6" spans="1:5" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="E7" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30.4" x14ac:dyDescent="0.35">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="E8" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30.4" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="E9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30.4" x14ac:dyDescent="0.35">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="E10" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30.4" x14ac:dyDescent="0.35">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12">
+      <c r="E11" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="101.25" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
-      <c r="B12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="10" t="s">
+      <c r="B12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="C12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" ht="42.75" customHeight="1">
+      <c r="D12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="121.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
-      <c r="C14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" ht="72.0" customHeight="1">
+      <c r="C14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="E15" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="101.25" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="B16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="C16" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="s">
+      <c r="D16" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="101.25" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18">
+      <c r="E17" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="81" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>47</v>
+      <c r="E18" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="C6:C11"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="D6:D11"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="A6:A12"/>
     <mergeCell ref="A13:A15"/>
@@ -923,13 +959,14 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="D6:D11"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
   </mergeCells>
-  <printOptions gridLines="1" horizontalCentered="1"/>
-  <pageMargins bottom="0.1" footer="0.0" header="0.0" left="0.1" right="0.1" top="0.1"/>
-  <pageSetup paperSize="9" cellComments="atEnd" orientation="portrait" pageOrder="overThenDown"/>
-  <drawing r:id="rId1"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.1" right="0.1" top="0.1" bottom="0.1" header="0" footer="0"/>
+  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" cellComments="atEnd"/>
 </worksheet>
 </file>
</xml_diff>